<commit_message>
feat: uses our need templates correctly
</commit_message>
<xml_diff>
--- a/data/Own_db/Our needs.xlsx
+++ b/data/Own_db/Our needs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rikde\PycharmProjects\FairyTale-Generator\data\Own_db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents-SSD\Interaction Technology\Natural Language Processing II\project\FairyTale-Generator\data\Own_db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027F467E-AEFA-4FC1-B67A-711B0A6F0F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2804196-3B78-487E-9CA5-F4165F9D7043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3A6F8556-8B22-4340-952F-3A1D945E21F8}"/>
+    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" xr2:uid="{3A6F8556-8B22-4340-952F-3A1D945E21F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Verb</t>
   </si>
@@ -42,40 +42,64 @@
     <t>Needs</t>
   </si>
   <si>
-    <t>are_disrespected_by</t>
-  </si>
-  <si>
-    <t>are_deceived_by</t>
-  </si>
-  <si>
     <t>kill</t>
   </si>
   <si>
-    <t>manipulate</t>
-  </si>
-  <si>
     <t>fall_in_love_with</t>
   </si>
   <si>
-    <t>profit_from</t>
-  </si>
-  <si>
-    <t>needs to get a reality check, wants to gain importance but should be more true to themselves, has to be humbled</t>
-  </si>
-  <si>
-    <t>needs to get a reality check, needs life change, has to be humbled</t>
-  </si>
-  <si>
-    <t>wants to catch B as they are very dangerous, wants to catch B as they pester everyone, wants to put an end to the history of terror that B is known for</t>
-  </si>
-  <si>
-    <t>wants control, wants to wield power/control (over someone?), wants to get rid of bad influence of B, wants someone to do their dirty work</t>
-  </si>
-  <si>
-    <t>wants to find true love, wants to find the love of their life, wants to get a companion, wants to find a partner, wants to search for love, wants to be loved, wants to no longer be alone, wants to change their opinion of B</t>
-  </si>
-  <si>
-    <t>wants to get further in life, wants to achieve more, wants to gain money, wants to become wealthy, wants to one-up B</t>
+    <t>doesn't know how bad B actually is, doesn't know about the evil that hides in B, doesn't know te bad side of B</t>
+  </si>
+  <si>
+    <t>steal_from</t>
+  </si>
+  <si>
+    <t>C find a treasure, C collect all the treasures in the world, C be even more rich and wealthy</t>
+  </si>
+  <si>
+    <t>C find true love, C find the love of their life, C get a companion, C find a partner, C search for love, C be loved, C no longer be alone, C change their opinion of B</t>
+  </si>
+  <si>
+    <t>are_feared_by</t>
+  </si>
+  <si>
+    <t>C be very powerful, C gain power, C be revered and admired</t>
+  </si>
+  <si>
+    <t>are_moved_by</t>
+  </si>
+  <si>
+    <t>C feel emotions again, C see beauty in the world, C experience true emotions</t>
+  </si>
+  <si>
+    <t>are_respected_by</t>
+  </si>
+  <si>
+    <t>C be admired, C be respected, C be looked upon with admiration</t>
+  </si>
+  <si>
+    <t>show_loyalty_to</t>
+  </si>
+  <si>
+    <t>C be loyal, C show B how much they mean to them, C find loyalty and devotion in their life</t>
+  </si>
+  <si>
+    <t>sleep_with</t>
+  </si>
+  <si>
+    <t>C be loved, C find a lover, C find romance in their life</t>
+  </si>
+  <si>
+    <t>turn_against</t>
+  </si>
+  <si>
+    <t>isn't aware of how bad B actually is, doesn't know about the evil that hides in B, doesn't know the bad side of B</t>
+  </si>
+  <si>
+    <t>testify_against</t>
+  </si>
+  <si>
+    <t>doesn't know the bad deeds B has done, isn't aware of the evil B is involved in, doesn't know the evil schemes B is involved in</t>
   </si>
 </sst>
 </file>
@@ -93,11 +117,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Roboto"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -440,19 +465,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1327F902-567C-4DDA-B256-D87A67761AA2}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="183.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="183.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,52 +485,84 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>